<commit_message>
[ADD] Fairness index for 5 Cubic added
</commit_message>
<xml_diff>
--- a/result/Jain_Fairness_index.xlsx
+++ b/result/Jain_Fairness_index.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imoni\Documents\NS3-BBR\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68169D9-17D0-473A-9356-FD1469B0F72A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76EDDA8-01C7-4C1C-87F5-A5548D5ED9C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A0475229-EA4A-4B5A-AD9A-CF41775D3558}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{A0475229-EA4A-4B5A-AD9A-CF41775D3558}"/>
   </bookViews>
   <sheets>
     <sheet name="3Cubic_2BBR" sheetId="1" r:id="rId1"/>
+    <sheet name="5Cubic_2BDP" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -47,6 +48,14 @@
       <sz val="8"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
@@ -73,8 +82,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1846,6 +1858,1754 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ko-KR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" baseline="0"/>
+              <a:t>5 CUBIC, 50M, 40ms, 2xBDP, time=(80, 90) </a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Cubic 1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'5Cubic_2BDP'!$A$1:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>80.001098999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80.500076000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>81.000504000000006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>81.500243999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>82.002303999999995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>82.500266999999994</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>83.000052999999994</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>83.500618000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>84.002135999999993</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>84.501357999999996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>85.000961000000004</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>85.501868999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>86.002243000000007</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>86.501236000000006</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>87.000488000000004</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>87.500748000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>88.000313000000006</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>88.500809000000004</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>89.001105999999993</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>89.500404000000003</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>90.000388999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'5Cubic_2BDP'!$B$1:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>10.856</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.815</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.688000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.54</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.7829999999999995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.08</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.292999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.433999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.585000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.688000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.763</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10.792</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10.79</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10.778</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10.71</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10.621</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.7519999999999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.8729999999999993</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10.042999999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10.176</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10.259</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0C0B-466A-8A93-4C64D57804AD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Cubic 2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'5Cubic_2BDP'!$D$1:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>80.001328000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80.502296000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>81.001694000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>81.501876999999993</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>82.000343000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>82.500031000000007</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>83.000861999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>83.500045999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>84.001105999999993</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>84.501129000000006</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>85.000656000000006</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>85.500450000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>86.000709999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>86.500731999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>87.001259000000005</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>87.500290000000007</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>88.000320000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>88.501343000000006</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>89.000602999999998</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>89.502396000000005</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>90.001159999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'5Cubic_2BDP'!$E$1:$E$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>10.443</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.355</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.356999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.3129999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.747</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.762</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.768000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.737</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.746</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.739000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.743</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10.714</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10.676</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10.664</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10.63</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10.586</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.7779999999999996</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>11.287000000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11.037000000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10.898999999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10.741</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0C0B-466A-8A93-4C64D57804AD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Cubic 3</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'5Cubic_2BDP'!$G$1:$G$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>80.000411999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80.500838999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>81.000275000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>81.501441999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>82.000113999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>82.500534000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>83.000290000000007</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>83.500290000000007</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>84.000145000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>84.500129999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>85.000923</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>85.500183000000007</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>86.000473</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>86.500236999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>87.000259</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>87.500518999999997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>88.000488000000004</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>88.501114000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>89.000336000000004</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>89.500168000000002</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>90.501686000000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'5Cubic_2BDP'!$H$1:$H$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>11.074</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.209</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.206</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.7919999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.037000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.621</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.340999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.09</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.9450000000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.8260000000000005</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.7799999999999994</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.7530000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9.7959999999999994</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.8659999999999997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10.013</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10.186</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.4930000000000003</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>11.009</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10.773999999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10.645</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10.396000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0C0B-466A-8A93-4C64D57804AD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>BBRv2 1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'5Cubic_2BDP'!$J$1:$J$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>80.000174999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80.500304999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>81.000045999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>81.502471999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>82.000290000000007</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>82.500534000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>83.000786000000005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>83.500313000000006</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>84.000373999999994</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>84.500304999999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>85.000427000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>85.500679000000005</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>86.000206000000006</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>86.500961000000004</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>87.000754999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>87.500052999999994</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>88.001045000000005</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>88.500572000000005</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>89.000107</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>89.501434000000003</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>90.000159999999994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'5Cubic_2BDP'!$K$1:$K$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>9.76</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.6110000000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.5030000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.64</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.087999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.018000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.9710000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.8919999999999995</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.8529999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.8119999999999994</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.7729999999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.75</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9.7200000000000006</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.7129999999999992</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9.7159999999999993</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.7210000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.98</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.5950000000000006</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9.6180000000000003</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.6590000000000007</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.6630000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-0C0B-466A-8A93-4C64D57804AD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>BBRv2 2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'5Cubic_2BDP'!$M$1:$M$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>80.000870000000006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80.500572000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>81.001464999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>81.500977000000006</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>82.001380999999995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>82.500800999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>83.003051999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>83.501075999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>84.000641000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>84.500359000000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>85.000152999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>85.500945999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>86.000938000000005</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>86.500504000000006</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>87.001564000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>87.500725000000003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>88.001273999999995</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>88.500076000000007</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>89.000832000000003</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>89.500670999999997</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>90.000327999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'5Cubic_2BDP'!$N$1:$N$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>6.7210000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.82</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.0049999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.1050000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.7539999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.7240000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.6879999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.62</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.5880000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.55</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.5140000000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.4859999999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.4740000000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.4790000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.5250000000000004</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.5869999999999997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7.7480000000000002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7.7439999999999998</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.7560000000000002</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.7169999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-0C0B-466A-8A93-4C64D57804AD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Total</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'5Cubic_2BDP'!$G$1:$G$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>80.000411999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80.500838999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>81.000275000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>81.501441999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>82.000113999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>82.500534000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>83.000290000000007</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>83.500290000000007</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>84.000145000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>84.500129999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>85.000923</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>85.500183000000007</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>86.000473</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>86.500236999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>87.000259</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>87.500518999999997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>88.000488000000004</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>88.501114000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>89.000336000000004</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>89.500168000000002</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>90.501686000000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'5Cubic_2BDP'!$P$1:$P$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>48.853999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>48.810000000000009</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>48.759000000000007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37.39</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49.408999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>49.204999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>49.061000000000007</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>48.772999999999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48.717000000000006</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>48.614999999999995</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>48.573</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>48.494999999999997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>48.456000000000003</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>48.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>48.594000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>48.701000000000008</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>35.503</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>49.511999999999993</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>49.216000000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>49.134999999999998</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>48.775999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-0C0B-466A-8A93-4C64D57804AD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="588756248"/>
+        <c:axId val="588751000"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="588756248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="90"/>
+          <c:min val="80"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="588751000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="588751000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="588756248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ko-KR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ko-KR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+                <a:latin typeface="+mn-ea"/>
+                <a:ea typeface="+mn-ea"/>
+              </a:rPr>
+              <a:t>5 CUBIC 50M, 40ms, 2xBDP, </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:latin typeface="+mn-ea"/>
+                <a:ea typeface="+mn-ea"/>
+              </a:rPr>
+              <a:t>Throughput Fairness Index</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="ko-KR" sz="1400">
+              <a:effectLst/>
+              <a:latin typeface="+mn-ea"/>
+              <a:ea typeface="+mn-ea"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'5Cubic_2BDP'!$M$24:$M$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>80.000870000000006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80.500572000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>81.001464999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>81.500977000000006</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>82.001380999999995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>82.500800999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>83.003051999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>83.501075999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>84.000641000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>84.500359000000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>85.000152999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>85.500945999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>86.000938000000005</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>86.500504000000006</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>87.001564000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>87.500725000000003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>88.001273999999995</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>88.500076000000007</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>89.000832000000003</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>89.500670999999997</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>90.000327999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'5Cubic_2BDP'!$P$24:$P$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0.97422456522823209</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.97497024711621083</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.97746079598359314</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.94640138692230436</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.98653728134980856</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.98770680092572971</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.98776711760219538</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98731087012775209</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9866718918145696</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.98601561615326327</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.98536760780270094</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.98507215259236647</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.98509554342580086</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.98523158688865309</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.98598693389565839</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.98683841726778554</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.98586802088836023</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.98418503572707894</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.98618000008199802</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.98720653403667458</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.98795935130716128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-04A7-4028-952B-00FE2EF69536}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1014555016"/>
+        <c:axId val="1319738496"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1014555016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="90"/>
+          <c:min val="80"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1319738496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1319738496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1014555016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ko-KR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1926,6 +3686,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2443,6 +4283,1038 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3019,6 +5891,87 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>270510</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>140970</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>355470</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>205290</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="차트 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FCA46E0-15DA-4D75-83FF-12468E49F2F4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>11430</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>294510</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>75750</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="차트 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82593B70-2ED3-4C2E-86D3-B2970CEC16CB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3334,7 +6287,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE4E9FB9-0F83-40CE-A6DA-86CD11CFA565}">
   <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="S27" sqref="S27"/>
     </sheetView>
   </sheetViews>
@@ -4857,4 +7810,1533 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45C243BE-5A5F-4D27-B98B-BC15285600B7}">
+  <dimension ref="A1:P44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A1" s="1">
+        <v>80.001098999999996</v>
+      </c>
+      <c r="B1" s="1">
+        <v>10.856</v>
+      </c>
+      <c r="D1">
+        <v>80.001328000000001</v>
+      </c>
+      <c r="E1">
+        <v>10.443</v>
+      </c>
+      <c r="G1">
+        <v>80.000411999999997</v>
+      </c>
+      <c r="H1">
+        <v>11.074</v>
+      </c>
+      <c r="J1">
+        <v>80.000174999999999</v>
+      </c>
+      <c r="K1">
+        <v>9.76</v>
+      </c>
+      <c r="M1">
+        <v>80.000870000000006</v>
+      </c>
+      <c r="N1">
+        <v>6.7210000000000001</v>
+      </c>
+      <c r="P1">
+        <f>SUM(B1,E1,H1,K1,N1)</f>
+        <v>48.853999999999999</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>80.500076000000007</v>
+      </c>
+      <c r="B2">
+        <v>10.815</v>
+      </c>
+      <c r="D2">
+        <v>80.502296000000001</v>
+      </c>
+      <c r="E2">
+        <v>10.355</v>
+      </c>
+      <c r="G2">
+        <v>80.500838999999999</v>
+      </c>
+      <c r="H2">
+        <v>11.209</v>
+      </c>
+      <c r="J2">
+        <v>80.500304999999997</v>
+      </c>
+      <c r="K2">
+        <v>9.6110000000000007</v>
+      </c>
+      <c r="M2">
+        <v>80.500572000000005</v>
+      </c>
+      <c r="N2">
+        <v>6.82</v>
+      </c>
+      <c r="P2">
+        <f t="shared" ref="P2:P21" si="0">SUM(B2,E2,H2,K2,N2)</f>
+        <v>48.810000000000009</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <v>81.000504000000006</v>
+      </c>
+      <c r="B3">
+        <v>10.688000000000001</v>
+      </c>
+      <c r="D3">
+        <v>81.001694000000001</v>
+      </c>
+      <c r="E3">
+        <v>10.356999999999999</v>
+      </c>
+      <c r="G3">
+        <v>81.000275000000002</v>
+      </c>
+      <c r="H3">
+        <v>11.206</v>
+      </c>
+      <c r="J3">
+        <v>81.000045999999998</v>
+      </c>
+      <c r="K3">
+        <v>9.5030000000000001</v>
+      </c>
+      <c r="M3">
+        <v>81.001464999999996</v>
+      </c>
+      <c r="N3">
+        <v>7.0049999999999999</v>
+      </c>
+      <c r="P3">
+        <f t="shared" si="0"/>
+        <v>48.759000000000007</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <v>81.500243999999995</v>
+      </c>
+      <c r="B4">
+        <v>10.54</v>
+      </c>
+      <c r="D4">
+        <v>81.501876999999993</v>
+      </c>
+      <c r="E4">
+        <v>7.3129999999999997</v>
+      </c>
+      <c r="G4">
+        <v>81.501441999999997</v>
+      </c>
+      <c r="H4">
+        <v>7.7919999999999998</v>
+      </c>
+      <c r="J4">
+        <v>81.502471999999997</v>
+      </c>
+      <c r="K4">
+        <v>6.64</v>
+      </c>
+      <c r="M4">
+        <v>81.500977000000006</v>
+      </c>
+      <c r="N4">
+        <v>5.1050000000000004</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="0"/>
+        <v>37.39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>82.002303999999995</v>
+      </c>
+      <c r="B5">
+        <v>9.7829999999999995</v>
+      </c>
+      <c r="D5">
+        <v>82.000343000000001</v>
+      </c>
+      <c r="E5">
+        <v>10.747</v>
+      </c>
+      <c r="G5">
+        <v>82.000113999999996</v>
+      </c>
+      <c r="H5">
+        <v>11.037000000000001</v>
+      </c>
+      <c r="J5">
+        <v>82.000290000000007</v>
+      </c>
+      <c r="K5">
+        <v>10.087999999999999</v>
+      </c>
+      <c r="M5">
+        <v>82.001380999999995</v>
+      </c>
+      <c r="N5">
+        <v>7.7539999999999996</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>49.408999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A6">
+        <v>82.500266999999994</v>
+      </c>
+      <c r="B6">
+        <v>10.08</v>
+      </c>
+      <c r="D6">
+        <v>82.500031000000007</v>
+      </c>
+      <c r="E6">
+        <v>10.762</v>
+      </c>
+      <c r="G6">
+        <v>82.500534000000002</v>
+      </c>
+      <c r="H6">
+        <v>10.621</v>
+      </c>
+      <c r="J6">
+        <v>82.500534000000002</v>
+      </c>
+      <c r="K6">
+        <v>10.018000000000001</v>
+      </c>
+      <c r="M6">
+        <v>82.500800999999996</v>
+      </c>
+      <c r="N6">
+        <v>7.7240000000000002</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="0"/>
+        <v>49.204999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A7">
+        <v>83.000052999999994</v>
+      </c>
+      <c r="B7">
+        <v>10.292999999999999</v>
+      </c>
+      <c r="D7">
+        <v>83.000861999999998</v>
+      </c>
+      <c r="E7">
+        <v>10.768000000000001</v>
+      </c>
+      <c r="G7">
+        <v>83.000290000000007</v>
+      </c>
+      <c r="H7">
+        <v>10.340999999999999</v>
+      </c>
+      <c r="J7">
+        <v>83.000786000000005</v>
+      </c>
+      <c r="K7">
+        <v>9.9710000000000001</v>
+      </c>
+      <c r="M7">
+        <v>83.003051999999997</v>
+      </c>
+      <c r="N7">
+        <v>7.6879999999999997</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="0"/>
+        <v>49.061000000000007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A8">
+        <v>83.500618000000003</v>
+      </c>
+      <c r="B8">
+        <v>10.433999999999999</v>
+      </c>
+      <c r="D8">
+        <v>83.500045999999998</v>
+      </c>
+      <c r="E8">
+        <v>10.737</v>
+      </c>
+      <c r="G8">
+        <v>83.500290000000007</v>
+      </c>
+      <c r="H8">
+        <v>10.09</v>
+      </c>
+      <c r="J8">
+        <v>83.500313000000006</v>
+      </c>
+      <c r="K8">
+        <v>9.8919999999999995</v>
+      </c>
+      <c r="M8">
+        <v>83.501075999999998</v>
+      </c>
+      <c r="N8">
+        <v>7.62</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="0"/>
+        <v>48.772999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A9">
+        <v>84.002135999999993</v>
+      </c>
+      <c r="B9">
+        <v>10.585000000000001</v>
+      </c>
+      <c r="D9">
+        <v>84.001105999999993</v>
+      </c>
+      <c r="E9">
+        <v>10.746</v>
+      </c>
+      <c r="G9">
+        <v>84.000145000000003</v>
+      </c>
+      <c r="H9">
+        <v>9.9450000000000003</v>
+      </c>
+      <c r="J9">
+        <v>84.000373999999994</v>
+      </c>
+      <c r="K9">
+        <v>9.8529999999999998</v>
+      </c>
+      <c r="M9">
+        <v>84.000641000000002</v>
+      </c>
+      <c r="N9">
+        <v>7.5880000000000001</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="0"/>
+        <v>48.717000000000006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A10">
+        <v>84.501357999999996</v>
+      </c>
+      <c r="B10">
+        <v>10.688000000000001</v>
+      </c>
+      <c r="D10">
+        <v>84.501129000000006</v>
+      </c>
+      <c r="E10">
+        <v>10.739000000000001</v>
+      </c>
+      <c r="G10">
+        <v>84.500129999999999</v>
+      </c>
+      <c r="H10">
+        <v>9.8260000000000005</v>
+      </c>
+      <c r="J10">
+        <v>84.500304999999997</v>
+      </c>
+      <c r="K10">
+        <v>9.8119999999999994</v>
+      </c>
+      <c r="M10">
+        <v>84.500359000000003</v>
+      </c>
+      <c r="N10">
+        <v>7.55</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="0"/>
+        <v>48.614999999999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A11">
+        <v>85.000961000000004</v>
+      </c>
+      <c r="B11">
+        <v>10.763</v>
+      </c>
+      <c r="D11">
+        <v>85.000656000000006</v>
+      </c>
+      <c r="E11">
+        <v>10.743</v>
+      </c>
+      <c r="G11">
+        <v>85.000923</v>
+      </c>
+      <c r="H11">
+        <v>9.7799999999999994</v>
+      </c>
+      <c r="J11">
+        <v>85.000427000000002</v>
+      </c>
+      <c r="K11">
+        <v>9.7729999999999997</v>
+      </c>
+      <c r="M11">
+        <v>85.000152999999997</v>
+      </c>
+      <c r="N11">
+        <v>7.5140000000000002</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="0"/>
+        <v>48.573</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A12">
+        <v>85.501868999999999</v>
+      </c>
+      <c r="B12">
+        <v>10.792</v>
+      </c>
+      <c r="D12">
+        <v>85.500450000000001</v>
+      </c>
+      <c r="E12">
+        <v>10.714</v>
+      </c>
+      <c r="G12">
+        <v>85.500183000000007</v>
+      </c>
+      <c r="H12">
+        <v>9.7530000000000001</v>
+      </c>
+      <c r="J12">
+        <v>85.500679000000005</v>
+      </c>
+      <c r="K12">
+        <v>9.75</v>
+      </c>
+      <c r="M12">
+        <v>85.500945999999999</v>
+      </c>
+      <c r="N12">
+        <v>7.4859999999999998</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="0"/>
+        <v>48.494999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A13">
+        <v>86.002243000000007</v>
+      </c>
+      <c r="B13">
+        <v>10.79</v>
+      </c>
+      <c r="D13">
+        <v>86.000709999999998</v>
+      </c>
+      <c r="E13">
+        <v>10.676</v>
+      </c>
+      <c r="G13">
+        <v>86.000473</v>
+      </c>
+      <c r="H13">
+        <v>9.7959999999999994</v>
+      </c>
+      <c r="J13">
+        <v>86.000206000000006</v>
+      </c>
+      <c r="K13">
+        <v>9.7200000000000006</v>
+      </c>
+      <c r="M13">
+        <v>86.000938000000005</v>
+      </c>
+      <c r="N13">
+        <v>7.4740000000000002</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="0"/>
+        <v>48.456000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A14">
+        <v>86.501236000000006</v>
+      </c>
+      <c r="B14">
+        <v>10.778</v>
+      </c>
+      <c r="D14">
+        <v>86.500731999999999</v>
+      </c>
+      <c r="E14">
+        <v>10.664</v>
+      </c>
+      <c r="G14">
+        <v>86.500236999999998</v>
+      </c>
+      <c r="H14">
+        <v>9.8659999999999997</v>
+      </c>
+      <c r="J14">
+        <v>86.500961000000004</v>
+      </c>
+      <c r="K14">
+        <v>9.7129999999999992</v>
+      </c>
+      <c r="M14">
+        <v>86.500504000000006</v>
+      </c>
+      <c r="N14">
+        <v>7.4790000000000001</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="0"/>
+        <v>48.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A15">
+        <v>87.000488000000004</v>
+      </c>
+      <c r="B15">
+        <v>10.71</v>
+      </c>
+      <c r="D15">
+        <v>87.001259000000005</v>
+      </c>
+      <c r="E15">
+        <v>10.63</v>
+      </c>
+      <c r="G15">
+        <v>87.000259</v>
+      </c>
+      <c r="H15">
+        <v>10.013</v>
+      </c>
+      <c r="J15">
+        <v>87.000754999999998</v>
+      </c>
+      <c r="K15">
+        <v>9.7159999999999993</v>
+      </c>
+      <c r="M15">
+        <v>87.001564000000002</v>
+      </c>
+      <c r="N15">
+        <v>7.5250000000000004</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="0"/>
+        <v>48.594000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A16">
+        <v>87.500748000000002</v>
+      </c>
+      <c r="B16">
+        <v>10.621</v>
+      </c>
+      <c r="D16">
+        <v>87.500290000000007</v>
+      </c>
+      <c r="E16">
+        <v>10.586</v>
+      </c>
+      <c r="G16">
+        <v>87.500518999999997</v>
+      </c>
+      <c r="H16">
+        <v>10.186</v>
+      </c>
+      <c r="J16">
+        <v>87.500052999999994</v>
+      </c>
+      <c r="K16">
+        <v>9.7210000000000001</v>
+      </c>
+      <c r="M16">
+        <v>87.500725000000003</v>
+      </c>
+      <c r="N16">
+        <v>7.5869999999999997</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="0"/>
+        <v>48.701000000000008</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A17">
+        <v>88.000313000000006</v>
+      </c>
+      <c r="B17">
+        <v>7.7519999999999998</v>
+      </c>
+      <c r="D17">
+        <v>88.000320000000002</v>
+      </c>
+      <c r="E17">
+        <v>7.7779999999999996</v>
+      </c>
+      <c r="G17">
+        <v>88.000488000000004</v>
+      </c>
+      <c r="H17">
+        <v>7.4930000000000003</v>
+      </c>
+      <c r="J17">
+        <v>88.001045000000005</v>
+      </c>
+      <c r="K17">
+        <v>6.98</v>
+      </c>
+      <c r="M17">
+        <v>88.001273999999995</v>
+      </c>
+      <c r="N17">
+        <v>5.5</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="0"/>
+        <v>35.503</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A18">
+        <v>88.500809000000004</v>
+      </c>
+      <c r="B18">
+        <v>9.8729999999999993</v>
+      </c>
+      <c r="D18">
+        <v>88.501343000000006</v>
+      </c>
+      <c r="E18">
+        <v>11.287000000000001</v>
+      </c>
+      <c r="G18">
+        <v>88.501114000000001</v>
+      </c>
+      <c r="H18">
+        <v>11.009</v>
+      </c>
+      <c r="J18">
+        <v>88.500572000000005</v>
+      </c>
+      <c r="K18">
+        <v>9.5950000000000006</v>
+      </c>
+      <c r="M18">
+        <v>88.500076000000007</v>
+      </c>
+      <c r="N18">
+        <v>7.7480000000000002</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="0"/>
+        <v>49.511999999999993</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A19">
+        <v>89.001105999999993</v>
+      </c>
+      <c r="B19">
+        <v>10.042999999999999</v>
+      </c>
+      <c r="D19">
+        <v>89.000602999999998</v>
+      </c>
+      <c r="E19">
+        <v>11.037000000000001</v>
+      </c>
+      <c r="G19">
+        <v>89.000336000000004</v>
+      </c>
+      <c r="H19">
+        <v>10.773999999999999</v>
+      </c>
+      <c r="J19">
+        <v>89.000107</v>
+      </c>
+      <c r="K19">
+        <v>9.6180000000000003</v>
+      </c>
+      <c r="M19">
+        <v>89.000832000000003</v>
+      </c>
+      <c r="N19">
+        <v>7.7439999999999998</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="0"/>
+        <v>49.216000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A20">
+        <v>89.500404000000003</v>
+      </c>
+      <c r="B20">
+        <v>10.176</v>
+      </c>
+      <c r="D20">
+        <v>89.502396000000005</v>
+      </c>
+      <c r="E20">
+        <v>10.898999999999999</v>
+      </c>
+      <c r="G20">
+        <v>89.500168000000002</v>
+      </c>
+      <c r="H20">
+        <v>10.645</v>
+      </c>
+      <c r="J20">
+        <v>89.501434000000003</v>
+      </c>
+      <c r="K20">
+        <v>9.6590000000000007</v>
+      </c>
+      <c r="M20">
+        <v>89.500670999999997</v>
+      </c>
+      <c r="N20">
+        <v>7.7560000000000002</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="0"/>
+        <v>49.134999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A21">
+        <v>90.000388999999998</v>
+      </c>
+      <c r="B21">
+        <v>10.259</v>
+      </c>
+      <c r="D21">
+        <v>90.001159999999999</v>
+      </c>
+      <c r="E21">
+        <v>10.741</v>
+      </c>
+      <c r="G21">
+        <v>90.501686000000007</v>
+      </c>
+      <c r="H21">
+        <v>10.396000000000001</v>
+      </c>
+      <c r="J21">
+        <v>90.000159999999994</v>
+      </c>
+      <c r="K21">
+        <v>9.6630000000000003</v>
+      </c>
+      <c r="M21">
+        <v>90.000327999999996</v>
+      </c>
+      <c r="N21">
+        <v>7.7169999999999996</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="0"/>
+        <v>48.775999999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A24" s="1">
+        <v>80.001098999999996</v>
+      </c>
+      <c r="B24" s="1">
+        <v>10.856</v>
+      </c>
+      <c r="D24">
+        <v>80.001328000000001</v>
+      </c>
+      <c r="E24">
+        <v>10.443</v>
+      </c>
+      <c r="G24">
+        <v>80.000411999999997</v>
+      </c>
+      <c r="H24">
+        <v>11.074</v>
+      </c>
+      <c r="J24">
+        <v>80.000174999999999</v>
+      </c>
+      <c r="K24">
+        <v>9.76</v>
+      </c>
+      <c r="M24">
+        <v>80.000870000000006</v>
+      </c>
+      <c r="N24">
+        <v>6.7210000000000001</v>
+      </c>
+      <c r="P24">
+        <f>(SUM(B24,E24,H24,K24,N24)^2)/(5*(B24^2+E24^2+H24^2+K24^2+N24^2))</f>
+        <v>0.97422456522823209</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A25">
+        <v>80.500076000000007</v>
+      </c>
+      <c r="B25">
+        <v>10.815</v>
+      </c>
+      <c r="D25">
+        <v>80.502296000000001</v>
+      </c>
+      <c r="E25">
+        <v>10.355</v>
+      </c>
+      <c r="G25">
+        <v>80.500838999999999</v>
+      </c>
+      <c r="H25">
+        <v>11.209</v>
+      </c>
+      <c r="J25">
+        <v>80.500304999999997</v>
+      </c>
+      <c r="K25">
+        <v>9.6110000000000007</v>
+      </c>
+      <c r="M25">
+        <v>80.500572000000005</v>
+      </c>
+      <c r="N25">
+        <v>6.82</v>
+      </c>
+      <c r="P25">
+        <f t="shared" ref="P25:P44" si="1">(SUM(B25,E25,H25,K25,N25)^2)/(5*(B25^2+E25^2+H25^2+K25^2+N25^2))</f>
+        <v>0.97497024711621083</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A26">
+        <v>81.000504000000006</v>
+      </c>
+      <c r="B26">
+        <v>10.688000000000001</v>
+      </c>
+      <c r="D26">
+        <v>81.001694000000001</v>
+      </c>
+      <c r="E26">
+        <v>10.356999999999999</v>
+      </c>
+      <c r="G26">
+        <v>81.000275000000002</v>
+      </c>
+      <c r="H26">
+        <v>11.206</v>
+      </c>
+      <c r="J26">
+        <v>81.000045999999998</v>
+      </c>
+      <c r="K26">
+        <v>9.5030000000000001</v>
+      </c>
+      <c r="M26">
+        <v>81.001464999999996</v>
+      </c>
+      <c r="N26">
+        <v>7.0049999999999999</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="1"/>
+        <v>0.97746079598359314</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A27">
+        <v>81.500243999999995</v>
+      </c>
+      <c r="B27">
+        <v>10.54</v>
+      </c>
+      <c r="D27">
+        <v>81.501876999999993</v>
+      </c>
+      <c r="E27">
+        <v>7.3129999999999997</v>
+      </c>
+      <c r="G27">
+        <v>81.501441999999997</v>
+      </c>
+      <c r="H27">
+        <v>7.7919999999999998</v>
+      </c>
+      <c r="J27">
+        <v>81.502471999999997</v>
+      </c>
+      <c r="K27">
+        <v>6.64</v>
+      </c>
+      <c r="M27">
+        <v>81.500977000000006</v>
+      </c>
+      <c r="N27">
+        <v>5.1050000000000004</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="1"/>
+        <v>0.94640138692230436</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A28">
+        <v>82.002303999999995</v>
+      </c>
+      <c r="B28">
+        <v>9.7829999999999995</v>
+      </c>
+      <c r="D28">
+        <v>82.000343000000001</v>
+      </c>
+      <c r="E28">
+        <v>10.747</v>
+      </c>
+      <c r="G28">
+        <v>82.000113999999996</v>
+      </c>
+      <c r="H28">
+        <v>11.037000000000001</v>
+      </c>
+      <c r="J28">
+        <v>82.000290000000007</v>
+      </c>
+      <c r="K28">
+        <v>10.087999999999999</v>
+      </c>
+      <c r="M28">
+        <v>82.001380999999995</v>
+      </c>
+      <c r="N28">
+        <v>7.7539999999999996</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="1"/>
+        <v>0.98653728134980856</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A29">
+        <v>82.500266999999994</v>
+      </c>
+      <c r="B29">
+        <v>10.08</v>
+      </c>
+      <c r="D29">
+        <v>82.500031000000007</v>
+      </c>
+      <c r="E29">
+        <v>10.762</v>
+      </c>
+      <c r="G29">
+        <v>82.500534000000002</v>
+      </c>
+      <c r="H29">
+        <v>10.621</v>
+      </c>
+      <c r="J29">
+        <v>82.500534000000002</v>
+      </c>
+      <c r="K29">
+        <v>10.018000000000001</v>
+      </c>
+      <c r="M29">
+        <v>82.500800999999996</v>
+      </c>
+      <c r="N29">
+        <v>7.7240000000000002</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="1"/>
+        <v>0.98770680092572971</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A30">
+        <v>83.000052999999994</v>
+      </c>
+      <c r="B30">
+        <v>10.292999999999999</v>
+      </c>
+      <c r="D30">
+        <v>83.000861999999998</v>
+      </c>
+      <c r="E30">
+        <v>10.768000000000001</v>
+      </c>
+      <c r="G30">
+        <v>83.000290000000007</v>
+      </c>
+      <c r="H30">
+        <v>10.340999999999999</v>
+      </c>
+      <c r="J30">
+        <v>83.000786000000005</v>
+      </c>
+      <c r="K30">
+        <v>9.9710000000000001</v>
+      </c>
+      <c r="M30">
+        <v>83.003051999999997</v>
+      </c>
+      <c r="N30">
+        <v>7.6879999999999997</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="1"/>
+        <v>0.98776711760219538</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A31">
+        <v>83.500618000000003</v>
+      </c>
+      <c r="B31">
+        <v>10.433999999999999</v>
+      </c>
+      <c r="D31">
+        <v>83.500045999999998</v>
+      </c>
+      <c r="E31">
+        <v>10.737</v>
+      </c>
+      <c r="G31">
+        <v>83.500290000000007</v>
+      </c>
+      <c r="H31">
+        <v>10.09</v>
+      </c>
+      <c r="J31">
+        <v>83.500313000000006</v>
+      </c>
+      <c r="K31">
+        <v>9.8919999999999995</v>
+      </c>
+      <c r="M31">
+        <v>83.501075999999998</v>
+      </c>
+      <c r="N31">
+        <v>7.62</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="1"/>
+        <v>0.98731087012775209</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A32">
+        <v>84.002135999999993</v>
+      </c>
+      <c r="B32">
+        <v>10.585000000000001</v>
+      </c>
+      <c r="D32">
+        <v>84.001105999999993</v>
+      </c>
+      <c r="E32">
+        <v>10.746</v>
+      </c>
+      <c r="G32">
+        <v>84.000145000000003</v>
+      </c>
+      <c r="H32">
+        <v>9.9450000000000003</v>
+      </c>
+      <c r="J32">
+        <v>84.000373999999994</v>
+      </c>
+      <c r="K32">
+        <v>9.8529999999999998</v>
+      </c>
+      <c r="M32">
+        <v>84.000641000000002</v>
+      </c>
+      <c r="N32">
+        <v>7.5880000000000001</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="1"/>
+        <v>0.9866718918145696</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A33">
+        <v>84.501357999999996</v>
+      </c>
+      <c r="B33">
+        <v>10.688000000000001</v>
+      </c>
+      <c r="D33">
+        <v>84.501129000000006</v>
+      </c>
+      <c r="E33">
+        <v>10.739000000000001</v>
+      </c>
+      <c r="G33">
+        <v>84.500129999999999</v>
+      </c>
+      <c r="H33">
+        <v>9.8260000000000005</v>
+      </c>
+      <c r="J33">
+        <v>84.500304999999997</v>
+      </c>
+      <c r="K33">
+        <v>9.8119999999999994</v>
+      </c>
+      <c r="M33">
+        <v>84.500359000000003</v>
+      </c>
+      <c r="N33">
+        <v>7.55</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="1"/>
+        <v>0.98601561615326327</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A34">
+        <v>85.000961000000004</v>
+      </c>
+      <c r="B34">
+        <v>10.763</v>
+      </c>
+      <c r="D34">
+        <v>85.000656000000006</v>
+      </c>
+      <c r="E34">
+        <v>10.743</v>
+      </c>
+      <c r="G34">
+        <v>85.000923</v>
+      </c>
+      <c r="H34">
+        <v>9.7799999999999994</v>
+      </c>
+      <c r="J34">
+        <v>85.000427000000002</v>
+      </c>
+      <c r="K34">
+        <v>9.7729999999999997</v>
+      </c>
+      <c r="M34">
+        <v>85.000152999999997</v>
+      </c>
+      <c r="N34">
+        <v>7.5140000000000002</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="1"/>
+        <v>0.98536760780270094</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A35">
+        <v>85.501868999999999</v>
+      </c>
+      <c r="B35">
+        <v>10.792</v>
+      </c>
+      <c r="D35">
+        <v>85.500450000000001</v>
+      </c>
+      <c r="E35">
+        <v>10.714</v>
+      </c>
+      <c r="G35">
+        <v>85.500183000000007</v>
+      </c>
+      <c r="H35">
+        <v>9.7530000000000001</v>
+      </c>
+      <c r="J35">
+        <v>85.500679000000005</v>
+      </c>
+      <c r="K35">
+        <v>9.75</v>
+      </c>
+      <c r="M35">
+        <v>85.500945999999999</v>
+      </c>
+      <c r="N35">
+        <v>7.4859999999999998</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="1"/>
+        <v>0.98507215259236647</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A36">
+        <v>86.002243000000007</v>
+      </c>
+      <c r="B36">
+        <v>10.79</v>
+      </c>
+      <c r="D36">
+        <v>86.000709999999998</v>
+      </c>
+      <c r="E36">
+        <v>10.676</v>
+      </c>
+      <c r="G36">
+        <v>86.000473</v>
+      </c>
+      <c r="H36">
+        <v>9.7959999999999994</v>
+      </c>
+      <c r="J36">
+        <v>86.000206000000006</v>
+      </c>
+      <c r="K36">
+        <v>9.7200000000000006</v>
+      </c>
+      <c r="M36">
+        <v>86.000938000000005</v>
+      </c>
+      <c r="N36">
+        <v>7.4740000000000002</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="1"/>
+        <v>0.98509554342580086</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A37">
+        <v>86.501236000000006</v>
+      </c>
+      <c r="B37">
+        <v>10.778</v>
+      </c>
+      <c r="D37">
+        <v>86.500731999999999</v>
+      </c>
+      <c r="E37">
+        <v>10.664</v>
+      </c>
+      <c r="G37">
+        <v>86.500236999999998</v>
+      </c>
+      <c r="H37">
+        <v>9.8659999999999997</v>
+      </c>
+      <c r="J37">
+        <v>86.500961000000004</v>
+      </c>
+      <c r="K37">
+        <v>9.7129999999999992</v>
+      </c>
+      <c r="M37">
+        <v>86.500504000000006</v>
+      </c>
+      <c r="N37">
+        <v>7.4790000000000001</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="1"/>
+        <v>0.98523158688865309</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A38">
+        <v>87.000488000000004</v>
+      </c>
+      <c r="B38">
+        <v>10.71</v>
+      </c>
+      <c r="D38">
+        <v>87.001259000000005</v>
+      </c>
+      <c r="E38">
+        <v>10.63</v>
+      </c>
+      <c r="G38">
+        <v>87.000259</v>
+      </c>
+      <c r="H38">
+        <v>10.013</v>
+      </c>
+      <c r="J38">
+        <v>87.000754999999998</v>
+      </c>
+      <c r="K38">
+        <v>9.7159999999999993</v>
+      </c>
+      <c r="M38">
+        <v>87.001564000000002</v>
+      </c>
+      <c r="N38">
+        <v>7.5250000000000004</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="1"/>
+        <v>0.98598693389565839</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A39">
+        <v>87.500748000000002</v>
+      </c>
+      <c r="B39">
+        <v>10.621</v>
+      </c>
+      <c r="D39">
+        <v>87.500290000000007</v>
+      </c>
+      <c r="E39">
+        <v>10.586</v>
+      </c>
+      <c r="G39">
+        <v>87.500518999999997</v>
+      </c>
+      <c r="H39">
+        <v>10.186</v>
+      </c>
+      <c r="J39">
+        <v>87.500052999999994</v>
+      </c>
+      <c r="K39">
+        <v>9.7210000000000001</v>
+      </c>
+      <c r="M39">
+        <v>87.500725000000003</v>
+      </c>
+      <c r="N39">
+        <v>7.5869999999999997</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="1"/>
+        <v>0.98683841726778554</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A40">
+        <v>88.000313000000006</v>
+      </c>
+      <c r="B40">
+        <v>7.7519999999999998</v>
+      </c>
+      <c r="D40">
+        <v>88.000320000000002</v>
+      </c>
+      <c r="E40">
+        <v>7.7779999999999996</v>
+      </c>
+      <c r="G40">
+        <v>88.000488000000004</v>
+      </c>
+      <c r="H40">
+        <v>7.4930000000000003</v>
+      </c>
+      <c r="J40">
+        <v>88.001045000000005</v>
+      </c>
+      <c r="K40">
+        <v>6.98</v>
+      </c>
+      <c r="M40">
+        <v>88.001273999999995</v>
+      </c>
+      <c r="N40">
+        <v>5.5</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="1"/>
+        <v>0.98586802088836023</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A41">
+        <v>88.500809000000004</v>
+      </c>
+      <c r="B41">
+        <v>9.8729999999999993</v>
+      </c>
+      <c r="D41">
+        <v>88.501343000000006</v>
+      </c>
+      <c r="E41">
+        <v>11.287000000000001</v>
+      </c>
+      <c r="G41">
+        <v>88.501114000000001</v>
+      </c>
+      <c r="H41">
+        <v>11.009</v>
+      </c>
+      <c r="J41">
+        <v>88.500572000000005</v>
+      </c>
+      <c r="K41">
+        <v>9.5950000000000006</v>
+      </c>
+      <c r="M41">
+        <v>88.500076000000007</v>
+      </c>
+      <c r="N41">
+        <v>7.7480000000000002</v>
+      </c>
+      <c r="P41">
+        <f t="shared" si="1"/>
+        <v>0.98418503572707894</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A42">
+        <v>89.001105999999993</v>
+      </c>
+      <c r="B42">
+        <v>10.042999999999999</v>
+      </c>
+      <c r="D42">
+        <v>89.000602999999998</v>
+      </c>
+      <c r="E42">
+        <v>11.037000000000001</v>
+      </c>
+      <c r="G42">
+        <v>89.000336000000004</v>
+      </c>
+      <c r="H42">
+        <v>10.773999999999999</v>
+      </c>
+      <c r="J42">
+        <v>89.000107</v>
+      </c>
+      <c r="K42">
+        <v>9.6180000000000003</v>
+      </c>
+      <c r="M42">
+        <v>89.000832000000003</v>
+      </c>
+      <c r="N42">
+        <v>7.7439999999999998</v>
+      </c>
+      <c r="P42">
+        <f t="shared" si="1"/>
+        <v>0.98618000008199802</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A43">
+        <v>89.500404000000003</v>
+      </c>
+      <c r="B43">
+        <v>10.176</v>
+      </c>
+      <c r="D43">
+        <v>89.502396000000005</v>
+      </c>
+      <c r="E43">
+        <v>10.898999999999999</v>
+      </c>
+      <c r="G43">
+        <v>89.500168000000002</v>
+      </c>
+      <c r="H43">
+        <v>10.645</v>
+      </c>
+      <c r="J43">
+        <v>89.501434000000003</v>
+      </c>
+      <c r="K43">
+        <v>9.6590000000000007</v>
+      </c>
+      <c r="M43">
+        <v>89.500670999999997</v>
+      </c>
+      <c r="N43">
+        <v>7.7560000000000002</v>
+      </c>
+      <c r="P43">
+        <f t="shared" si="1"/>
+        <v>0.98720653403667458</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A44">
+        <v>90.000388999999998</v>
+      </c>
+      <c r="B44">
+        <v>10.259</v>
+      </c>
+      <c r="D44">
+        <v>90.001159999999999</v>
+      </c>
+      <c r="E44">
+        <v>10.741</v>
+      </c>
+      <c r="G44">
+        <v>90.501686000000007</v>
+      </c>
+      <c r="H44">
+        <v>10.396000000000001</v>
+      </c>
+      <c r="J44">
+        <v>90.000159999999994</v>
+      </c>
+      <c r="K44">
+        <v>9.6630000000000003</v>
+      </c>
+      <c r="M44">
+        <v>90.000327999999996</v>
+      </c>
+      <c r="N44">
+        <v>7.7169999999999996</v>
+      </c>
+      <c r="P44">
+        <f t="shared" si="1"/>
+        <v>0.98795935130716128</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[FIX] new assets added and time range of results fixed
</commit_message>
<xml_diff>
--- a/result/Jain_Fairness_index.xlsx
+++ b/result/Jain_Fairness_index.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imoni\Documents\NS3-BBR\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76EDDA8-01C7-4C1C-87F5-A5548D5ED9C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F9DA63-E7DA-4FB0-86F1-CFCB4BC58DB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{A0475229-EA4A-4B5A-AD9A-CF41775D3558}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A0475229-EA4A-4B5A-AD9A-CF41775D3558}"/>
   </bookViews>
   <sheets>
     <sheet name="3Cubic_2BBR" sheetId="1" r:id="rId1"/>
@@ -140,14 +140,23 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" altLang="ko-KR"/>
+              <a:rPr lang="en-US" altLang="ko-KR">
+                <a:latin typeface="+mn-ea"/>
+                <a:ea typeface="+mn-ea"/>
+              </a:rPr>
               <a:t>3</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" altLang="ko-KR" baseline="0"/>
+              <a:rPr lang="en-US" altLang="ko-KR" baseline="0">
+                <a:latin typeface="+mn-ea"/>
+                <a:ea typeface="+mn-ea"/>
+              </a:rPr>
               <a:t> CUBIC 2 BBRv2, 50M, 40ms, 2xBDP, time=(80, 90) </a:t>
             </a:r>
-            <a:endParaRPr lang="ko-KR" altLang="en-US"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US">
+              <a:latin typeface="+mn-ea"/>
+              <a:ea typeface="+mn-ea"/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -5840,10 +5849,10 @@
       <xdr:rowOff>140970</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>355470</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>205290</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>94350</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>66270</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5876,10 +5885,10 @@
       <xdr:rowOff>11430</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>294510</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>75750</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>33390</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>157710</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6287,8 +6296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE4E9FB9-0F83-40CE-A6DA-86CD11CFA565}">
   <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="S27" sqref="S27"/>
+    <sheetView tabSelected="1" topLeftCell="R19" workbookViewId="0">
+      <selection activeCell="AG28" sqref="AG28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -7816,7 +7825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45C243BE-5A5F-4D27-B98B-BC15285600B7}">
   <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>

</xml_diff>